<commit_message>
Update test results data - 2025-04-12 05:19 PM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 6.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\FBS Result Giver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\DU FBS Mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AD081C-FD47-47F7-A939-D676AF1A2A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CBA418-9939-4065-B8DC-713AA6BE371D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="Z24" sqref="Z24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF26" si="14">_xlfn.RANK.EQ(AE2, $AE$2:$AE$1002, 0)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AG2" s="13"/>
       <c r="AH2">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="Y3">
         <f t="shared" si="12"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Z3" s="20">
         <v>7</v>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="AF3">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AG3" s="13"/>
       <c r="AH3">
@@ -1592,28 +1592,52 @@
       <c r="B4" s="11" t="s">
         <v>38</v>
       </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12.25</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>76.5625</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="J4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>79.166666666666657</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>6</v>
       </c>
       <c r="M4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="N4">
         <f t="shared" si="5"/>
+        <v>40.625</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
@@ -1624,25 +1648,31 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
+      <c r="S4">
+        <v>12</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
       <c r="U4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>11.25</v>
       </c>
       <c r="V4">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>70.3125</v>
       </c>
       <c r="W4">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>E4 + I4 + M4 +Q4+U4</f>
+        <v>39.5</v>
       </c>
       <c r="X4">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>65.833333333333329</v>
       </c>
       <c r="Y4">
         <f t="shared" si="12"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="Z4" s="20">
         <v>8</v>
@@ -1659,11 +1689,11 @@
       </c>
       <c r="AE4">
         <f t="shared" si="13"/>
-        <v>32</v>
+        <v>71.5</v>
       </c>
       <c r="AF4">
         <f t="shared" si="14"/>
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="AG4" s="13"/>
       <c r="AH4">
@@ -1757,7 +1787,7 @@
       </c>
       <c r="Y5">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Z5" s="20">
         <v>6.5</v>
@@ -1778,7 +1808,7 @@
       </c>
       <c r="AF5">
         <f t="shared" si="14"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG5" s="13"/>
       <c r="AH5">
@@ -1872,7 +1902,7 @@
       </c>
       <c r="Y6">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z6" s="20">
         <v>6</v>
@@ -1893,7 +1923,7 @@
       </c>
       <c r="AF6">
         <f t="shared" si="14"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AH6">
         <f>SUM(AH1:AH5)</f>
@@ -1987,7 +2017,7 @@
       </c>
       <c r="Y7">
         <f t="shared" si="12"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z7" s="20">
         <v>8</v>
@@ -2008,7 +2038,7 @@
       </c>
       <c r="AF7">
         <f t="shared" si="14"/>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2098,7 +2128,7 @@
       </c>
       <c r="Y8">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z8" s="19">
         <v>7</v>
@@ -2119,7 +2149,7 @@
       </c>
       <c r="AF8">
         <f t="shared" si="14"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AI8">
         <v>-0.25</v>
@@ -2182,7 +2212,7 @@
       </c>
       <c r="Y9">
         <f t="shared" si="12"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z9" s="22"/>
       <c r="AA9" s="21"/>
@@ -2255,7 +2285,7 @@
       </c>
       <c r="Y10">
         <f t="shared" si="12"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z10" s="21"/>
       <c r="AA10" s="21"/>
@@ -2358,7 +2388,7 @@
       </c>
       <c r="Y11">
         <f t="shared" si="12"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Z11" s="20">
         <v>6.5</v>
@@ -2379,7 +2409,7 @@
       </c>
       <c r="AF11">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2486,7 +2516,7 @@
       </c>
       <c r="AF12">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2576,7 +2606,7 @@
       </c>
       <c r="Y13">
         <f t="shared" si="12"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Z13" s="19">
         <v>6.5</v>
@@ -2597,7 +2627,7 @@
       </c>
       <c r="AF13">
         <f t="shared" si="14"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2768,7 +2798,7 @@
       </c>
       <c r="Y15">
         <f t="shared" si="12"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z15" s="21"/>
       <c r="AA15" s="21"/>
@@ -2841,7 +2871,7 @@
       </c>
       <c r="Y16">
         <f t="shared" si="12"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z16" s="21"/>
       <c r="AA16" s="21"/>
@@ -2914,7 +2944,7 @@
       </c>
       <c r="Y17">
         <f t="shared" si="12"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z17" s="21"/>
       <c r="AA17" s="21"/>
@@ -2987,7 +3017,7 @@
       </c>
       <c r="Y18">
         <f t="shared" si="12"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Z18" s="21"/>
       <c r="AA18" s="21"/>
@@ -3090,7 +3120,7 @@
       </c>
       <c r="Y19">
         <f t="shared" si="12"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z19" s="20">
         <v>8.5</v>
@@ -3111,7 +3141,7 @@
       </c>
       <c r="AF19">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3122,18 +3152,18 @@
         <v>70</v>
       </c>
       <c r="C20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>13.75</v>
+        <v>15</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
-        <v>85.9375</v>
+        <v>93.75</v>
       </c>
       <c r="G20">
         <v>9</v>
@@ -3193,15 +3223,15 @@
       </c>
       <c r="W20">
         <f t="shared" si="10"/>
-        <v>40.75</v>
+        <v>42</v>
       </c>
       <c r="X20">
         <f t="shared" si="11"/>
-        <v>67.916666666666671</v>
+        <v>70</v>
       </c>
       <c r="Y20">
         <f t="shared" si="12"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z20" s="20">
         <v>6.5</v>
@@ -3218,11 +3248,11 @@
       </c>
       <c r="AE20">
         <f t="shared" si="13"/>
-        <v>67.25</v>
+        <v>68.5</v>
       </c>
       <c r="AF20">
         <f t="shared" si="14"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3333,7 +3363,7 @@
       </c>
       <c r="AF21">
         <f t="shared" si="14"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3423,7 +3453,7 @@
       </c>
       <c r="Y22">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Z22" s="20">
         <v>8</v>
@@ -3444,7 +3474,7 @@
       </c>
       <c r="AF22">
         <f t="shared" si="14"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3658,7 +3688,7 @@
       </c>
       <c r="AF24">
         <f t="shared" si="14"/>
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="43.8" thickBot="1">
@@ -3880,7 +3910,7 @@
       </c>
       <c r="AF26">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:32">

</xml_diff>

<commit_message>
Update test results data - 2025-04-12 05:57 PM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 6.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\DU FBS Mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CBA418-9939-4065-B8DC-713AA6BE371D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D91687-3EF4-461C-934C-E3D7C98B61A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1246,7 +1246,7 @@
   <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="AF4">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG4" s="13"/>
       <c r="AH4">
@@ -2501,8 +2501,12 @@
         <f t="shared" si="12"/>
         <v>2</v>
       </c>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="21"/>
+      <c r="Z12" s="21">
+        <v>6</v>
+      </c>
+      <c r="AA12" s="21">
+        <v>7.5</v>
+      </c>
       <c r="AB12" s="20">
         <v>8.5</v>
       </c>
@@ -2512,11 +2516,11 @@
       </c>
       <c r="AE12">
         <f t="shared" si="13"/>
-        <v>68.25</v>
+        <v>81.75</v>
       </c>
       <c r="AF12">
         <f t="shared" si="14"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2738,7 +2742,7 @@
       </c>
       <c r="AF14">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -3252,7 +3256,7 @@
       </c>
       <c r="AF20">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3799,7 +3803,7 @@
       </c>
       <c r="AF25">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="29.4" thickBot="1">

</xml_diff>

<commit_message>
Update test results data - 2025-04-12 06:05 PM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 6.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\DU FBS Mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D91687-3EF4-461C-934C-E3D7C98B61A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11B5DDC-901E-4CDF-9272-A78819D682DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -1245,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="80" workbookViewId="0">
       <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
@@ -4977,11 +4977,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BZ26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5644,6 +5644,196 @@
       <c r="B4" s="15" t="s">
         <v>38</v>
       </c>
+      <c r="C4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="S4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="U4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="V4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="W4" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="X4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA4" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB4" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AD4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="AE4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="AH4" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="AI4" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ4" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="AK4" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL4" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="18"/>
+      <c r="AO4" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="AP4" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="AQ4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AR4" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AS4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="AT4" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="AU4" s="18"/>
+      <c r="AV4" s="18"/>
+      <c r="AW4" s="18"/>
+      <c r="AX4" s="18"/>
+      <c r="AY4" s="18"/>
+      <c r="AZ4" s="18"/>
+      <c r="BA4" s="18"/>
+      <c r="BB4" s="18"/>
+      <c r="BC4" s="18"/>
+      <c r="BD4" s="18"/>
+      <c r="BE4" s="18"/>
+      <c r="BF4" s="18"/>
+      <c r="BG4" s="18"/>
+      <c r="BH4" s="18"/>
+      <c r="BI4" s="18"/>
+      <c r="BJ4" s="18"/>
+      <c r="BK4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BL4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="BM4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BN4" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="BO4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BP4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="BQ4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="BR4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BS4" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="BT4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="BU4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BV4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="BW4" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX4" s="18"/>
+      <c r="BY4" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="BZ4" s="16" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="5" spans="1:78">
       <c r="A5" s="15" t="s">

</xml_diff>